<commit_message>
Added feature that equally distributes tickets to chosen agents after the all the agents with priority are full
</commit_message>
<xml_diff>
--- a/zoho.xlsx
+++ b/zoho.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Departments" sheetId="2" r:id="rId2"/>
+    <sheet name="Main Orig" sheetId="3" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
@@ -398,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -414,19 +415,22 @@
         <v>Order (by ID)</v>
       </c>
       <c r="D1" t="str">
+        <v>Priority On/Off</v>
+      </c>
+      <c r="E1" t="str">
         <v>Total Tickets Max</v>
       </c>
-      <c r="E1" t="str">
+      <c r="F1" t="str">
         <v>Waiting on Us Tickets Max</v>
       </c>
-      <c r="F1" t="str">
+      <c r="G1" t="str">
         <v>Number of Tickets Assigned Currently</v>
       </c>
-      <c r="I1" t="str">
+      <c r="J1" t="str">
         <v>Department:</v>
       </c>
-      <c r="J1" t="str">
-        <v>Modix</v>
+      <c r="K1" t="str">
+        <v>Sandbox</v>
       </c>
     </row>
     <row r="2">
@@ -439,21 +443,24 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>100</v>
+      <c r="D2" t="str">
+        <v>t</v>
       </c>
       <c r="E2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>78</v>
-      </c>
-      <c r="I2" t="str">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="str">
         <v>ID:</v>
       </c>
-      <c r="J2" t="str">
-        <f>VLOOKUP(Main!J1,Departments!A2:B10,2,FALSE)</f>
-        <v>846378000000006907</v>
+      <c r="K2" t="str">
+        <f>VLOOKUP(Main!K1,Departments!A2:B10,2,FALSE)</f>
+        <v>846378000000705029</v>
       </c>
     </row>
     <row r="3">
@@ -466,14 +473,17 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3">
-        <v>25</v>
+      <c r="D3" t="str">
+        <v>t</v>
       </c>
       <c r="E3">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>25</v>
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -486,14 +496,17 @@
       <c r="C4">
         <v>2</v>
       </c>
-      <c r="D4">
-        <v>0</v>
+      <c r="D4" t="str">
+        <v>t</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -506,14 +519,17 @@
       <c r="C5">
         <v>3</v>
       </c>
-      <c r="D5">
-        <v>30</v>
+      <c r="D5" t="str">
+        <v>f</v>
       </c>
       <c r="E5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>17</v>
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -526,14 +542,17 @@
       <c r="C6">
         <v>4</v>
       </c>
-      <c r="D6">
-        <v>30</v>
+      <c r="D6" t="str">
+        <v>f</v>
       </c>
       <c r="E6">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>14</v>
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -546,40 +565,23 @@
       <c r="C7">
         <v>5</v>
       </c>
-      <c r="D7">
-        <v>30</v>
+      <c r="D7" t="str">
+        <v>f</v>
       </c>
       <c r="E7">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>Shachar  Gafni</v>
-      </c>
-      <c r="B8">
-        <v>6</v>
-      </c>
-      <c r="C8">
-        <v>6</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K7"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -621,4 +623,192 @@
     <ignoredError numberStoredAsText="1" sqref="A1:B3"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Agent Name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>Agent ID</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Order (by ID)</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Total Tickets Max</v>
+      </c>
+      <c r="E1" t="str">
+        <v>Waiting on Us Tickets Max</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Number of Tickets Assigned Currently</v>
+      </c>
+      <c r="I1" t="str">
+        <v>Department:</v>
+      </c>
+      <c r="J1" t="str">
+        <v>Modix</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Lazar Jovic</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>78</v>
+      </c>
+      <c r="I2" t="str">
+        <v>ID:</v>
+      </c>
+      <c r="J2" t="str">
+        <f>VLOOKUP('Main Orig'!J1,Departments!A2:B10,2,FALSE)</f>
+        <v>846378000000006907</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Max Sobolev</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>25</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Oleg Yermanok</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Omri Gazit</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>30</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>On Zoarezh</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="str">
+        <v>x</v>
+      </c>
+      <c r="D6">
+        <v>30</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Saar Neufeld</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="str">
+        <v>x</v>
+      </c>
+      <c r="D7">
+        <v>30</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Shachar  Gafni</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="str">
+        <v>x</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:J8"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>